<commit_message>
Änderungen in Köln am 3.10.2025
</commit_message>
<xml_diff>
--- a/Börse FLow.xlsx
+++ b/Börse FLow.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://consulting42-my.sharepoint.com/personal/helmut_consulting42_onmicrosoft_com/Documents/Desktop Austausch/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Helmut\AppData\Roaming\MetaQuotes\Terminal\870072DB5DBAB61841BAE146AFAAFB8A\MQL5\Experts\Winner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="11_AD4DB114E441178AC67DF4AB0E15F51E693EDF10" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58A395B2-F625-480F-85A1-45B732DAEC1D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E197A9-C63D-4DF7-B90D-0EA2566FA79A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21072" yWindow="288" windowWidth="20556" windowHeight="12324" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21072" yWindow="72" windowWidth="20556" windowHeight="12324" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Ereignis</t>
   </si>
@@ -88,6 +88,15 @@
   </si>
   <si>
     <t>NeuerDreierNeu(ID)</t>
+  </si>
+  <si>
+    <t>BarClose(timeframe) - 1</t>
+  </si>
+  <si>
+    <t>NeuerDreierNeu(ID) - 2</t>
+  </si>
+  <si>
+    <t>DreierKaputt(ID) - 3</t>
   </si>
 </sst>
 </file>
@@ -429,7 +438,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -485,7 +494,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>6</v>
@@ -509,7 +518,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>9</v>
@@ -525,7 +534,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Änderung am 2025-10-06 19:39
</commit_message>
<xml_diff>
--- a/Börse FLow.xlsx
+++ b/Börse FLow.xlsx
@@ -8,25 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Helmut\AppData\Roaming\MetaQuotes\Terminal\870072DB5DBAB61841BAE146AFAAFB8A\MQL5\Experts\Winner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B72128A-226C-4844-8E7B-4468AB9616A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534580D2-DA4E-46F0-A118-7B03849A8A2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20616" yWindow="12" windowWidth="20556" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20916" yWindow="-120" windowWidth="20220" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="94">
   <si>
     <t>Ereignis</t>
   </si>
@@ -136,18 +147,12 @@
     <t>Array (PatternID,Art,Status,time0,price0)</t>
   </si>
   <si>
-    <t>PatternNeu</t>
-  </si>
-  <si>
     <t>EntryNeu</t>
   </si>
   <si>
     <t>EntryUpd</t>
   </si>
   <si>
-    <t>PatternUpd</t>
-  </si>
-  <si>
     <t>BarClose</t>
   </si>
   <si>
@@ -160,9 +165,6 @@
     <t>offene Pattern prüfen ggf. UPD</t>
   </si>
   <si>
-    <t>neue Bars?  Alte Bar Schliessen</t>
-  </si>
-  <si>
     <t>ggf. neue Pattern</t>
   </si>
   <si>
@@ -191,12 +193,6 @@
   </si>
   <si>
     <t>Pattern   n:1   Enrires   1:n   Positionen   1:3-5 Orders</t>
-  </si>
-  <si>
-    <t>ggf neue Entries errechnen</t>
-  </si>
-  <si>
-    <t>lfd entries ändern</t>
   </si>
   <si>
     <t>ggf Entry änderung errechnen</t>
@@ -331,70 +327,73 @@
     </r>
   </si>
   <si>
-    <t>patternId;</t>
-  </si>
-  <si>
-    <t>timeFrame;</t>
-  </si>
-  <si>
-    <t>art;</t>
-  </si>
-  <si>
-    <t>richtung;</t>
-  </si>
-  <si>
-    <t>id;</t>
-  </si>
-  <si>
-    <t>typ;</t>
-  </si>
-  <si>
-    <t>time;</t>
-  </si>
-  <si>
-    <t>level;</t>
-  </si>
-  <si>
-    <t>pkt1;</t>
-  </si>
-  <si>
-    <t>status;</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> = pattern [patternIdx2].</t>
-  </si>
-  <si>
-    <t>pattern [patternIdx1].</t>
-  </si>
-  <si>
-    <t>patternId</t>
-  </si>
-  <si>
-    <t>timeFrame</t>
-  </si>
-  <si>
-    <t>art</t>
-  </si>
-  <si>
-    <t>richtung</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>typ</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>level</t>
-  </si>
-  <si>
-    <t>pkt1</t>
-  </si>
-  <si>
-    <t>status</t>
+    <t>PatternNeu(Typ)</t>
+  </si>
+  <si>
+    <t>H1: neue Entries errechnen</t>
+  </si>
+  <si>
+    <t>(lfd entries ändern)</t>
+  </si>
+  <si>
+    <t>PatternUpd(patternId)</t>
+  </si>
+  <si>
+    <t>neuer Bar?  Alter Bar schliessen</t>
+  </si>
+  <si>
+    <t>ok - neuer Bar?  Alter Bar schliessen</t>
+  </si>
+  <si>
+    <t>ggf. neue Pattern. Welche?</t>
+  </si>
+  <si>
+    <t>`* Prüfung auf Rng aus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Aufruf BarCLose </t>
+  </si>
+  <si>
+    <t>* lfd Bars mit .last versorgen</t>
+  </si>
+  <si>
+    <t>DreierStatus</t>
+  </si>
+  <si>
+    <t>ang</t>
+  </si>
+  <si>
+    <t>off</t>
+  </si>
+  <si>
+    <t>tkp</t>
+  </si>
+  <si>
+    <t>kpt</t>
+  </si>
+  <si>
+    <t>fake</t>
+  </si>
+  <si>
+    <t>aus</t>
+  </si>
+  <si>
+    <t>3er</t>
+  </si>
+  <si>
+    <t>PatternTyp</t>
+  </si>
+  <si>
+    <t>* Dreier ang tkp ?</t>
+  </si>
+  <si>
+    <t>* Range</t>
+  </si>
+  <si>
+    <t>* tkp =&gt; kpt oder fake</t>
+  </si>
+  <si>
+    <t>* 3er kpt = ? Trenjdbruch</t>
   </si>
 </sst>
 </file>
@@ -425,7 +424,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -435,6 +434,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -460,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -477,10 +482,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -763,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -802,167 +811,166 @@
         <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C10" s="5"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>39</v>
+      <c r="A15" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>59</v>
+      <c r="C23" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
-      <c r="C24" s="6"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>59</v>
+      <c r="C25" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="36" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -977,7 +985,7 @@
         <v>5</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -987,7 +995,7 @@
     </row>
     <row r="36" spans="1:3" ht="36" x14ac:dyDescent="0.3">
       <c r="B36" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="36" x14ac:dyDescent="0.3">
@@ -995,12 +1003,12 @@
         <v>7</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="54" x14ac:dyDescent="0.3">
       <c r="B39" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="54" x14ac:dyDescent="0.3">
@@ -1011,7 +1019,7 @@
         <v>9</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -1035,7 +1043,7 @@
         <v>10</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>35</v>
@@ -1046,10 +1054,10 @@
         <v>32</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="54" x14ac:dyDescent="0.3">
@@ -1070,22 +1078,22 @@
         <v>13</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="B55" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B56" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B58" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -1100,7 +1108,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B61" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
@@ -1156,7 +1164,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B75" s="3"/>
     </row>
@@ -1168,156 +1176,203 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19006EF1-E3C5-4393-865D-A2DD1C9ECD46}">
-  <dimension ref="C8:F17"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="C8:F17"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="46.5546875" customWidth="1"/>
     <col min="3" max="3" width="24.88671875" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C8" s="7" t="s">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" t="s">
         <v>87</v>
       </c>
-      <c r="D8" t="s">
-        <v>88</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C9" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C10" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D10" t="s">
-        <v>90</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C11" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D11" t="s">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C8" s="6"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C9" s="6"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C12" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C13" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="C13" s="5"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C15" s="6"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="B21" s="9" t="s">
         <v>93</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C14" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D14" t="s">
-        <v>94</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C15" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D15" t="s">
-        <v>95</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C16" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D16" t="s">
-        <v>96</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C17" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D17" t="s">
-        <v>97</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F17" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enry strukur[1;5D[1;5D[1;5D[1;5D[D[D[D[D[D[Dtry struc incl order – am 2025-10-08 11:38
</commit_message>
<xml_diff>
--- a/Börse FLow.xlsx
+++ b/Börse FLow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Helmut\AppData\Roaming\MetaQuotes\Terminal\870072DB5DBAB61841BAE146AFAAFB8A\MQL5\Experts\Winner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534580D2-DA4E-46F0-A118-7B03849A8A2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0A0858-909A-4300-BC39-EBCEB70DE567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20916" yWindow="-120" windowWidth="20220" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="264" yWindow="60" windowWidth="20220" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="98">
   <si>
     <t>Ereignis</t>
   </si>
@@ -135,9 +135,6 @@
     <t>&gt;&gt; Tick *Börse</t>
   </si>
   <si>
-    <t>Position</t>
-  </si>
-  <si>
     <t xml:space="preserve">Zur Realisierung einer Position senden wir eine Kauf/Verkauf-Order mit ZusatzInfo an die Börse. </t>
   </si>
   <si>
@@ -171,25 +168,10 @@
     <t>Posiitonsmgr lfd Orders</t>
   </si>
   <si>
-    <t>alte Posiitonen sperren</t>
-  </si>
-  <si>
-    <t>Neue Positionenerrechnen</t>
-  </si>
-  <si>
-    <t>PositionsNeu</t>
-  </si>
-  <si>
     <t>PositionsUpd</t>
   </si>
   <si>
-    <t>Positionen loeschen; Hier und Börse</t>
-  </si>
-  <si>
     <t>Orders an die Börse</t>
-  </si>
-  <si>
-    <t>SL oder TP Order ändern; Orders löschen</t>
   </si>
   <si>
     <t>Pattern   n:1   Enrires   1:n   Positionen   1:3-5 Orders</t>
@@ -333,9 +315,6 @@
     <t>H1: neue Entries errechnen</t>
   </si>
   <si>
-    <t>(lfd entries ändern)</t>
-  </si>
-  <si>
     <t>PatternUpd(patternId)</t>
   </si>
   <si>
@@ -394,6 +373,39 @@
   </si>
   <si>
     <t>* 3er kpt = ? Trenjdbruch</t>
+  </si>
+  <si>
+    <t>H1: alte Entries löschen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suchen alle M3 3er: Nach H1 Anfang;  im H1 Frame; </t>
+  </si>
+  <si>
+    <t>in H1-Pattern-Richtung und auch tiefster TB</t>
+  </si>
+  <si>
+    <t>alle off Entries unterhalb aus</t>
+  </si>
+  <si>
+    <t>Alte Entries deaktiv</t>
+  </si>
+  <si>
+    <t>Level Korrektur</t>
+  </si>
+  <si>
+    <t>Löschen: Orders wegnehmen</t>
+  </si>
+  <si>
+    <t>SL;TP änderung</t>
+  </si>
+  <si>
+    <t>PatternNeu(#)</t>
+  </si>
+  <si>
+    <t>PatternUpd(#)</t>
+  </si>
+  <si>
+    <t>Orders für alle offenen Entries bilden</t>
   </si>
 </sst>
 </file>
@@ -487,7 +499,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -770,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C75"/>
+  <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -806,367 +818,346 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="B9" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B13" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B15" s="2" t="s">
+    </row>
+    <row r="27" spans="1:3" ht="36" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:3" ht="54" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B33" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="36" x14ac:dyDescent="0.3">
+      <c r="B34" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B16" s="2" t="s">
+    </row>
+    <row r="36" spans="1:3" ht="36" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B19" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="2" t="s">
+    </row>
+    <row r="37" spans="1:3" ht="54" x14ac:dyDescent="0.3">
+      <c r="B37" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="5"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="36" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="1:3" ht="54" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B35" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="36" x14ac:dyDescent="0.3">
-      <c r="B36" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="36" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
     <row r="39" spans="1:3" ht="54" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="B39" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="54" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B41" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C39" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B40" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="54" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="B42" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="54" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="54" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B46" s="2" t="s">
+    <row r="45" spans="1:3" ht="90" x14ac:dyDescent="0.3">
+      <c r="B45" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="54" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="B48" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="36" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="B52" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="90" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B48" s="2" t="s">
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B53" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B55" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="54" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="B51" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="36" x14ac:dyDescent="0.3">
-      <c r="A53" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="B55" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B56" s="2" t="s">
-        <v>66</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B57" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B58" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B59" s="2" t="s">
-        <v>15</v>
+      <c r="B58" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="B60" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B61" s="3" t="s">
-        <v>70</v>
+      <c r="B61" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B62" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="B63" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B64" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B65" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B66" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="B67" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B68" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B71" s="2" t="s">
         <v>28</v>
       </c>
     </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B69" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B72" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B75" s="3"/>
+      <c r="A72" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B72" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1176,10 +1167,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19006EF1-E3C5-4393-865D-A2DD1C9ECD46}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1195,75 +1186,75 @@
         <v>31</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="8" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="8" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" t="s">
         <v>77</v>
-      </c>
-      <c r="E4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E6" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E7" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1276,72 +1267,55 @@
     </row>
     <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="8" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
-      <c r="B13" s="6" t="s">
-        <v>92</v>
+      <c r="B13" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="C13" s="5"/>
       <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" s="5"/>
       <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C15" s="6"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>36</v>
-      </c>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>37</v>
-      </c>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.3">
@@ -1352,27 +1326,62 @@
     </row>
     <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="B21" s="9" t="s">
-        <v>93</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="B25" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Änderung am 2025-10-13 15:20  auf HelmutsLaptop
</commit_message>
<xml_diff>
--- a/Börse FLow.xlsx
+++ b/Börse FLow.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Helmut\AppData\Roaming\MetaQuotes\Terminal\870072DB5DBAB61841BAE146AFAAFB8A\MQL5\Experts\Winner\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mail\AppData\Roaming\MetaQuotes\Terminal\911BA40074322CF56CA471EE108EBB30\MQL5\Experts\Winner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0A0858-909A-4300-BC39-EBCEB70DE567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5574706-D4C5-46D6-ABD0-A0224E50159A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="264" yWindow="60" windowWidth="20220" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="100">
   <si>
     <t>Ereignis</t>
   </si>
@@ -407,12 +407,18 @@
   <si>
     <t>Orders für alle offenen Entries bilden</t>
   </si>
+  <si>
+    <t xml:space="preserve">Level Korrektur:  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  alte linien für Peeks;  GAPs, Dojis im Level</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -430,6 +436,13 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -477,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -500,6 +513,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -784,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -1167,9 +1183,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19006EF1-E3C5-4393-865D-A2DD1C9ECD46}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -1362,7 +1378,7 @@
     </row>
     <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="10" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1384,7 +1400,27 @@
         <v>89</v>
       </c>
     </row>
+    <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A30" s="2"/>
+      <c r="B30" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="B32" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Änderung am 2025-10-14 15:55
</commit_message>
<xml_diff>
--- a/Börse FLow.xlsx
+++ b/Börse FLow.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mail\AppData\Roaming\MetaQuotes\Terminal\911BA40074322CF56CA471EE108EBB30\MQL5\Experts\Winner\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Helmut\AppData\Roaming\MetaQuotes\Terminal\870072DB5DBAB61841BAE146AFAAFB8A\MQL5\Experts\Winner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5574706-D4C5-46D6-ABD0-A0224E50159A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967C0FC3-ED8F-4011-8CBE-6D94A9E81B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20676" yWindow="276" windowWidth="20220" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="107">
   <si>
     <t>Ereignis</t>
   </si>
@@ -187,9 +187,6 @@
   </si>
   <si>
     <t>Order Status geändern/Loeschen</t>
-  </si>
-  <si>
-    <t>Lfd Orders Stoppen?       Dateien schreiben: Pattern; Entries; Positionen</t>
   </si>
   <si>
     <t xml:space="preserve">Ein Satz aus dem Datenfeed T&amp;S( Time und Sales) der Börse, der über einen abgeschlossenen Deal dort informiert.   </t>
@@ -412,6 +409,30 @@
   </si>
   <si>
     <t xml:space="preserve">  alte linien für Peeks;  GAPs, Dojis im Level</t>
+  </si>
+  <si>
+    <t>22 Uhr</t>
+  </si>
+  <si>
+    <t>Entries: lfd Orders close</t>
+  </si>
+  <si>
+    <t>07 Uhr</t>
+  </si>
+  <si>
+    <t>Entries verdichten ("off","hdl","aus")</t>
+  </si>
+  <si>
+    <t>off  Entries zeichnen  (Zeichenprogramm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lfd Orders Stoppen?     </t>
+  </si>
+  <si>
+    <t>Pattern; Entries: Versichten und Scheiben</t>
+  </si>
+  <si>
+    <t>Positonsmgr lfd Orders</t>
   </si>
 </sst>
 </file>
@@ -798,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C72"/>
+  <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:B20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -836,7 +857,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -844,7 +865,7 @@
         <v>31</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>37</v>
@@ -855,7 +876,7 @@
         <v>41</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -863,7 +884,7 @@
         <v>40</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -874,7 +895,7 @@
         <v>41</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -882,21 +903,23 @@
         <v>40</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>35</v>
@@ -904,7 +927,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>36</v>
@@ -912,7 +935,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>46</v>
@@ -934,20 +957,21 @@
         <v>35</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="C20" s="5"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>48</v>
@@ -955,7 +979,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>48</v>
@@ -963,7 +987,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>49</v>
@@ -972,208 +996,237 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="36" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>59</v>
+        <v>99</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-    </row>
-    <row r="32" spans="1:3" ht="54" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B28" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>51</v>
+        <v>104</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B33" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+    </row>
+    <row r="36" spans="1:3" ht="54" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B37" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="36" x14ac:dyDescent="0.3">
-      <c r="B34" s="2" t="s">
+    <row r="38" spans="1:3" ht="36" x14ac:dyDescent="0.3">
+      <c r="B38" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="36" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="36" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" s="2" t="s">
+    <row r="41" spans="1:3" ht="54" x14ac:dyDescent="0.3">
+      <c r="B41" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="54" x14ac:dyDescent="0.3">
-      <c r="B37" s="2" t="s">
+    <row r="43" spans="1:3" ht="54" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B44" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="54" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="54" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="54" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B40" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="54" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
+      <c r="C48" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="90" x14ac:dyDescent="0.3">
+      <c r="B49" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="54" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="B52" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="36" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="B56" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B57" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B59" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B60" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B61" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B62" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="54" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="90" x14ac:dyDescent="0.3">
-      <c r="B45" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="54" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="B48" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="36" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="B52" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B53" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B55" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B56" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B57" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B58" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B60" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B61" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B62" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B63" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B64" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B65" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B66" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="B67" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B68" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B69" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B72" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B73" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" s="4" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B72" s="3"/>
+      <c r="B76" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1185,7 +1238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19006EF1-E3C5-4393-865D-A2DD1C9ECD46}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -1202,51 +1255,51 @@
         <v>31</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.3">
@@ -1254,23 +1307,23 @@
         <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1289,14 +1342,14 @@
         <v>41</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E11" s="6"/>
     </row>
@@ -1306,14 +1359,14 @@
         <v>40</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C13" s="5"/>
       <c r="E13" s="6"/>
@@ -1342,7 +1395,7 @@
     </row>
     <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>46</v>
@@ -1362,15 +1415,15 @@
     </row>
     <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="B21" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>36</v>
@@ -1379,12 +1432,12 @@
     <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>35</v>
@@ -1392,12 +1445,12 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.3">
@@ -1405,13 +1458,13 @@
         <v>35</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="18" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Änderung am 2025-10-20 19:39  auf HelmutsLaptop
</commit_message>
<xml_diff>
--- a/Börse FLow.xlsx
+++ b/Börse FLow.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Helmut\AppData\Roaming\MetaQuotes\Terminal\870072DB5DBAB61841BAE146AFAAFB8A\MQL5\Experts\Winner\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mail\AppData\Roaming\MetaQuotes\Terminal\911BA40074322CF56CA471EE108EBB30\MQL5\Experts\Winner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967C0FC3-ED8F-4011-8CBE-6D94A9E81B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D64EFC-B750-45B1-9B8A-4F11FAB5298C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20676" yWindow="276" windowWidth="20220" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2124" yWindow="492" windowWidth="19656" windowHeight="11364" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
+    <sheet name="Für Markus" sheetId="3" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId2"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="164">
   <si>
     <t>Ereignis</t>
   </si>
@@ -434,12 +435,297 @@
   <si>
     <t>Positonsmgr lfd Orders</t>
   </si>
+  <si>
+    <t>Verarbeitung</t>
+  </si>
+  <si>
+    <t>Neuer Deal an der Börse</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Börse sendet uns  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NewTick</t>
+    </r>
+  </si>
+  <si>
+    <t>NewTick (time,price,volumen)</t>
+  </si>
+  <si>
+    <t>Bemerkung</t>
+  </si>
+  <si>
+    <t>Wir arbeiten mit vier "Time Frames"  D1 = 24 h  H1 = 60 min  M3 = 3min M1 = 1min</t>
+  </si>
+  <si>
+    <t>anfangszeit, open, high, low close, volumen</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Call  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NewBar</t>
+    </r>
+  </si>
+  <si>
+    <t>NewBar (timeFrame)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nehme die 3 alten Bars des timeframes und prüfe ob </t>
+  </si>
+  <si>
+    <t>die zusammen ein Pattern  machen. Wenn ja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pattern in Liste der Pattern (Patternart, timeframe, </t>
+  </si>
+  <si>
+    <t>anfangszeit,  Eigenschaften)</t>
+  </si>
+  <si>
+    <t>NewPattern(patternID)</t>
+  </si>
+  <si>
+    <t>Call NewPattern(PatternID = uniqueKey)</t>
+  </si>
+  <si>
+    <t>Prüfungen je nach timeFrame und PatternArt</t>
+  </si>
+  <si>
+    <t>dazu andere Pattern lesen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">evtl. neuer Entry gefunden. </t>
+  </si>
+  <si>
+    <t>NewEntry(entryID)</t>
+  </si>
+  <si>
+    <t>ggf. lfd Trade beenden. Offenen orders an der Börse löschen</t>
+  </si>
+  <si>
+    <t>Tick gegen alle (noch offenen) Pattern prüfen</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Call </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ChangeBar</t>
+    </r>
+  </si>
+  <si>
+    <t>pro timeFrame: Gehört der Tick noch zum Bar?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> s o n st </t>
+  </si>
+  <si>
+    <t>aktuellen Bars anpassen: max high, min low,close, vol+</t>
+  </si>
+  <si>
+    <t>Tick gegen alle (noch offenen) Entries  prüfen)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bars im timeframe rollen und neuen Bar öffnen mit </t>
+  </si>
+  <si>
+    <t>Change Bar(timeFrame)</t>
+  </si>
+  <si>
+    <t>NewOrder(OrderID)</t>
+  </si>
+  <si>
+    <t>PatternZustandGeändert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ggf.  Zustand des Pattern ändern </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Call </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PatternZustandGeändert</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ggf.  Zustand des Entry ändern </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Eintragen in Liste der Entries Call </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NewEntry</t>
+    </r>
+  </si>
+  <si>
+    <t>Order gefüllt an der Börse</t>
+  </si>
+  <si>
+    <t>Börse sendet uns FILL</t>
+  </si>
+  <si>
+    <t>FILL (OrderID)</t>
+  </si>
+  <si>
+    <t>Fill zeigt an:  OrderFill oder StopFill  oder TP1Fill oder TP2FIll?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">call </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FillEntry</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>um 22 Uhr Tzagesabschluss: off Order schliessen, statistiken schreiben usw</t>
+  </si>
+  <si>
+    <t>EntryDeaktivieren(entryID)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">andere Entries löschen call </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> EntryDeaktivieren</t>
+    </r>
+  </si>
+  <si>
+    <t>B örse sendet jetzt oder Minuten odr Stunden später</t>
+  </si>
+  <si>
+    <t>FillOrder(time, Price, volumen)</t>
+  </si>
+  <si>
+    <t>Order an die Börse senden (tatsächlich 4 orders)</t>
+  </si>
+  <si>
+    <t>FillSL oder FILL TP1  odr FIllTP2.</t>
+  </si>
+  <si>
+    <t>Börse sendet Quittung oder Fehler</t>
+  </si>
+  <si>
+    <t>NewOrder (ok, Nok) angenommen abgelehnt</t>
+  </si>
+  <si>
+    <t>was mache ich da?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In jedem Time Frame werden die Ticks zu Bars zusammen gefasst. </t>
+  </si>
+  <si>
+    <t>Ein Bar im timeframe H1 geht also z.B. von 8:00  Uhr bis 9 Uhr (8:00 Uhr bis 08:59  und 59,99 sekunden)</t>
+  </si>
+  <si>
+    <t>Ein Bar speichert nicht alle Ticks sondern nur</t>
+  </si>
+  <si>
+    <t>die Anfangszeit, den ersten Price = open, den höchsten in der Zeitspanne = high, low, den letzten =  close, und das Gesamt volumen)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Call </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EntryZustandGeändert</t>
+    </r>
+  </si>
+  <si>
+    <t>Wir halten in jedem Time Frame 3 alte und einen aktuellen Bar für die Pattern erkennung</t>
+  </si>
+  <si>
+    <t>timer sendet Zeitsignal um 8 Uhr, 9 Uhr, 22 Uhr oder Newstab</t>
+  </si>
+  <si>
+    <t>22:00 Uhr</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -469,8 +755,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -486,6 +780,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -511,7 +811,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -539,6 +839,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -818,10 +1120,301 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EE66C80-67A9-405B-AAE9-AED28B23F453}">
+  <dimension ref="A1:C57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33" customWidth="1"/>
+    <col min="2" max="2" width="44.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>115</v>
+      </c>
+      <c r="B18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B24" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>134</v>
+      </c>
+      <c r="B26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>120</v>
+      </c>
+      <c r="B28" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B33" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>125</v>
+      </c>
+      <c r="B38" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>147</v>
+      </c>
+      <c r="B45" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>135</v>
+      </c>
+      <c r="B48" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>141</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>143</v>
+      </c>
+      <c r="B52" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>163</v>
+      </c>
+      <c r="B57" t="s">
+        <v>146</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -1234,7 +1827,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19006EF1-E3C5-4393-865D-A2DD1C9ECD46}">
   <dimension ref="A1:E32"/>
   <sheetViews>

</xml_diff>

<commit_message>
Änderung am 2025-10-28 15:07  auf HelmutsLaptop
</commit_message>
<xml_diff>
--- a/Börse FLow.xlsx
+++ b/Börse FLow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mail\AppData\Roaming\MetaQuotes\Terminal\911BA40074322CF56CA471EE108EBB30\MQL5\Experts\Winner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CB3BD8-3031-4903-A3E8-DC9C114574FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B91117-00A6-4456-9563-B8F1A6725FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="348" yWindow="456" windowWidth="22692" windowHeight="11364" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ereignisse" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="129">
   <si>
     <t>Was haben wir hier?</t>
   </si>
@@ -416,9 +416,6 @@
     <t>Level-Korrektur</t>
   </si>
   <si>
-    <t>wenn B1 oder B2 dDoji</t>
-  </si>
-  <si>
     <t>die zusammen ein Pattern  machen. Wenn ja Pattern in Patternarray eintragen</t>
   </si>
   <si>
@@ -458,9 +455,6 @@
     <t>Trade/Position</t>
   </si>
   <si>
-    <t xml:space="preserve">Beginnt mit einer Einstiegsorder. Der Trade immer durch eine Stoporder, die den Verlust begrenzt, und eine TakeProfit Order begrenzt.  Gem den Regeln für das Positionsmanagement können Einheiten dazu oder weg genommen werden. Ich bezeichne die Aktionen von der Position "FLAT" zur Position "FLAT" als Trade.  Je nach RIchtung die Einstiegsorder, ist man LONG (Gewinn bei steigenden Kursen) oder SHORT (Gewinn bei fallenden Krusen) positioniert. </t>
-  </si>
-  <si>
     <t>Wir senden Buy oder Sell Orders an die Börse. Die Orders haben Ausführungsregeln: Markt; Limit; Stop Orders für die Realisierung des SL und des TP sollten OCO (one cancel the other) verbunden sein. (Tatsächlich kennt die Börse nur Mrket und Limit. Es ist der Broker, der Stop und OCO ausführt).</t>
   </si>
   <si>
@@ -470,9 +464,6 @@
     <t xml:space="preserve">Andere Chartformen fassen immer mehrere Ticks zusammen indem sie den ersten, den höchsten, tiefsten und den letzten Preis einer Einheit in einer grafischer Form zusammenfassen. Wir nutzen die Darstellungsform  "BarChart". Für die Zusammenfassung werden Zeit- oder Volumen-Einheiten genutzt. Wir nutzen neben den Tickchart (Darstellungsform: Linienchart) nur sog. time-based Charts. </t>
   </si>
   <si>
-    <t>In Charts ergeben sich Muster (Pattern) die Rückschlüsse auf das Geschehen am Markt zulsássen..</t>
-  </si>
-  <si>
     <t>??? Noch unklar ???</t>
   </si>
   <si>
@@ -485,9 +476,6 @@
     <t>Handelsrichtung</t>
   </si>
   <si>
-    <t>Wir handeln von H1 Level zu H1 Level. Mit dem Anhandeln eines off M3-3er in einem off H1-3er dreht sich die Richtung. Wenn der Krus einen H1-3er kaputt macht, dreht sich die Richtung.</t>
-  </si>
-  <si>
     <t>* * *</t>
   </si>
   <si>
@@ -501,9 +489,6 @@
   </si>
   <si>
     <t>Handelsrichtung drehen</t>
-  </si>
-  <si>
-    <t>Trend und Handelsrichtung</t>
   </si>
   <si>
     <t>Wenn Bar 2 Doji dann Level drüber</t>
@@ -526,6 +511,33 @@
   </si>
   <si>
     <t>Wi egenau geht  ggf. Neuer H1Break-Entry erzeugen</t>
+  </si>
+  <si>
+    <t>Wenn GAP dann Level drüber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trend vs SZ bestimmen; ;Offene Entries lesen; Lfd Orders an der Börse; lesen; Zusammenführen; </t>
+  </si>
+  <si>
+    <t>Trend;Handelsrichtung und SZ</t>
+  </si>
+  <si>
+    <t>SZ Schiebezone bestimmen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schiebezone (SZ) </t>
+  </si>
+  <si>
+    <t>Läuft der Markt in einem Trend oder schiebt er seitlich</t>
+  </si>
+  <si>
+    <t>In Charts ergeben sich Muster (Pattern) die Rückschlüsse auf das Geschehen am Markt zulassen..</t>
+  </si>
+  <si>
+    <t>Wir handeln von H1 Level zu H1 Level. Mit dem Anhandeln eines off M3-3er in einem off H1-3er dreht sich die Richtung. Wenn der Kurs einen H1-3er kaputt macht, dreht sich die Richtung.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beginnt mit einer Einstiegsorder. Der Trade immer durch eine Stoporder, die den Verlust begrenzt, und eine TakeProfit Order begrenzt.  Gem den Regeln für das Positionsmanagement können Einheiten dazu oder weg genommen werden. Ich bezeichne die Aktionen von der Position "FLAT" zur Position "FLAT" als Trade.  Je nach RIchtung die Einstiegsorder, ist man LONG (Gewinn bei steigenden Kursen) oder SHORT (Gewinn bei fallenden Kursen) positioniert. </t>
   </si>
 </sst>
 </file>
@@ -630,7 +642,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -915,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81131D85-7CD5-46A3-93C6-A82BB3D6DEF5}">
   <dimension ref="A1:WYY34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -938,7 +950,7 @@
         <v>8</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>10</v>
@@ -961,7 +973,7 @@
         <v>47</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -972,7 +984,7 @@
         <v>48</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1032,10 +1044,13 @@
         <v>86</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>121</v>
+      </c>
       <c r="C7" s="6" t="s">
         <v>23</v>
       </c>
@@ -1046,7 +1061,7 @@
         <v>90</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1057,16 +1072,16 @@
         <v>61</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>72</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1080,7 +1095,7 @@
         <v>73</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1091,10 +1106,10 @@
         <v>74</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1108,7 +1123,7 @@
         <v>75</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1119,7 +1134,7 @@
         <v>55</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="6" t="s">
@@ -1137,7 +1152,7 @@
         <v>76</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>26</v>
@@ -1152,7 +1167,10 @@
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="6" t="s">
-        <v>119</v>
+        <v>115</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>123</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>31</v>
@@ -1160,7 +1178,7 @@
     </row>
     <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>80</v>
@@ -1171,7 +1189,7 @@
     </row>
     <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>84</v>
@@ -1195,7 +1213,7 @@
     <row r="19" spans="1:6 16223:16223" ht="18" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="D19" s="6" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="WYY19" s="6">
         <v>7</v>
@@ -1206,7 +1224,7 @@
         <v>60</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:6 16223:16223" ht="15.6" x14ac:dyDescent="0.3">
@@ -1225,7 +1243,7 @@
         <v>21</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>24</v>
@@ -1234,7 +1252,7 @@
     <row r="23" spans="1:6 16223:16223" ht="18" x14ac:dyDescent="0.3">
       <c r="C23" s="1"/>
       <c r="D23" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>30</v>
@@ -1242,13 +1260,13 @@
     </row>
     <row r="24" spans="1:6 16223:16223" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D24" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:6 16223:16223" ht="18" x14ac:dyDescent="0.3">
       <c r="C25" s="1"/>
       <c r="D25" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:6 16223:16223" ht="18" x14ac:dyDescent="0.3">
@@ -1290,10 +1308,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE2D9C1-3F89-42F4-954D-C084D654A421}">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41:B42"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B33" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1319,7 +1337,7 @@
     <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.3">
@@ -1349,13 +1367,13 @@
     <row r="8" spans="1:2" ht="90" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="36" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.3">
@@ -1415,129 +1433,125 @@
         <v>9</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:2" ht="54" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
+        <v>125</v>
+      </c>
     </row>
     <row r="23" spans="1:2" ht="54" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>3</v>
+        <v>111</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>69</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="1:2" ht="108" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="54" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>105</v>
+        <v>3</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>106</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="108" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>4</v>
+        <v>104</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:2" ht="18" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>5</v>
+    <row r="29" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>15</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="1:2" ht="36" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
+    <row r="31" spans="1:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="B31" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
-      <c r="B32" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="1:2" ht="36" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
+      <c r="B33" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="34" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
-      <c r="B35" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B35" s="1"/>
     </row>
     <row r="36" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
-      <c r="B37" s="2" t="s">
-        <v>16</v>
+      <c r="B37" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
+      <c r="B38" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="39" spans="1:2" ht="18" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B39" s="1"/>
+      <c r="A39" s="1"/>
+      <c r="B39" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="40" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
     </row>
     <row r="41" spans="1:2" ht="18" x14ac:dyDescent="0.3">
-      <c r="A41" s="1"/>
+      <c r="A41" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="B41" s="1"/>
     </row>
     <row r="42" spans="1:2" ht="18" x14ac:dyDescent="0.3">
@@ -1557,7 +1571,7 @@
       <c r="B45" s="1"/>
     </row>
     <row r="46" spans="1:2" ht="18" x14ac:dyDescent="0.3">
-      <c r="A46" s="2"/>
+      <c r="A46" s="1"/>
       <c r="B46" s="1"/>
     </row>
     <row r="47" spans="1:2" ht="18" x14ac:dyDescent="0.3">
@@ -1565,7 +1579,7 @@
       <c r="B47" s="1"/>
     </row>
     <row r="48" spans="1:2" ht="18" x14ac:dyDescent="0.3">
-      <c r="A48" s="1"/>
+      <c r="A48" s="2"/>
       <c r="B48" s="1"/>
     </row>
     <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.3">
@@ -1577,12 +1591,20 @@
       <c r="B50" s="1"/>
     </row>
     <row r="51" spans="1:2" ht="18" x14ac:dyDescent="0.3">
-      <c r="A51" s="3"/>
-      <c r="B51" s="2"/>
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
     </row>
     <row r="52" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
+    </row>
+    <row r="53" spans="1:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="A53" s="3"/>
+      <c r="B53" s="2"/>
+    </row>
+    <row r="54" spans="1:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>